<commit_message>
calculate rate of ART initiation overtime
</commit_message>
<xml_diff>
--- a/param_files/ART_initiation_rate.xlsx
+++ b/param_files/ART_initiation_rate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/Google Drive/HIV:TB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/ws/github/epi_model_HIV_TB/param_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22674C86-FAF6-5747-BDD7-EEE81018DEA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71237A75-4C0E-FB42-BA3E-F08D875AB6C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17640" yWindow="1060" windowWidth="10000" windowHeight="15500" xr2:uid="{23E87AAA-F98F-6E44-8E92-6D3127C9E120}"/>
+    <workbookView xWindow="8080" yWindow="1060" windowWidth="19560" windowHeight="15500" xr2:uid="{23E87AAA-F98F-6E44-8E92-6D3127C9E120}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <r>
       <t>ART coverage over time by gender</t>
@@ -51,132 +51,6 @@
     <t>Females </t>
   </si>
   <si>
-    <r>
-      <t>2004</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2005</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF222222"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2006</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2007</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF222222"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2008</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2009</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF222222"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2010</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2011</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF222222"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2017</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
     <t>HIV -</t>
   </si>
   <si>
@@ -221,12 +95,6 @@
     </r>
   </si>
   <si>
-    <t>https://serve.mg.co.za/content/documents/2018/07/17/7M1RBtUShKFJbN3NL1Wr_HSRC_HIV_Survey_Summary_2018.pdf</t>
-  </si>
-  <si>
-    <t>http://repository.hsrc.ac.za/bitstream/handle/20.500.11910/2490/8162.pdf?sequence=1&amp;is</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -384,26 +252,19 @@
   </si>
   <si>
     <t>7.0–12.4</t>
-  </si>
-  <si>
-    <t>r&amp;$a2/KnS!pSCTA</t>
-  </si>
-  <si>
-    <t>page 37?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;????_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -417,12 +278,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -452,6 +307,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -476,15 +352,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -495,16 +372,19 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -816,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD3C5C0-7259-F74C-B74F-4B62E66F4BA2}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,28 +714,28 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -873,8 +753,8 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" s="2">
+        <v>2004</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -882,32 +762,37 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="13">
-        <f>1-H3</f>
-        <v>0.7</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0.3</v>
+      <c r="F3" s="1">
+        <v>2005</v>
+      </c>
+      <c r="G3" s="16">
+        <f t="shared" ref="G3:G10" si="0">1-H3</f>
+        <v>0.86170000000000002</v>
+      </c>
+      <c r="H3" s="16">
+        <f>VLOOKUP(F3,$A$16:$B$28,2)*0.01</f>
+        <v>0.13830000000000001</v>
       </c>
       <c r="I3" s="4">
-        <f>B3</f>
-        <v>0</v>
+        <f>VLOOKUP(F3,$A$3:$C$11,2)</f>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="J3" s="7">
-        <f>$N$2*H3</f>
-        <v>30000</v>
+        <f t="shared" ref="J3:J10" si="1">$N$2*H3</f>
+        <v>13830</v>
       </c>
       <c r="K3" s="6">
         <f>I3*J3</f>
-        <v>0</v>
+        <v>78.831000000000003</v>
+      </c>
+      <c r="L3" s="8">
+        <f>(K3-0)/J3</f>
+        <v>5.7000000000000002E-3</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
+      <c r="A4" s="1">
+        <v>2005</v>
       </c>
       <c r="B4">
         <v>5.7000000000000002E-3</v>
@@ -915,36 +800,37 @@
       <c r="C4">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="13">
-        <f t="shared" ref="G4:G11" si="0">1-H4</f>
-        <v>0.7</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0.3</v>
+      <c r="F4" s="2">
+        <v>2006</v>
+      </c>
+      <c r="G4" s="16">
+        <f t="shared" si="0"/>
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="H4" s="16">
+        <f t="shared" ref="H4:H10" si="2">VLOOKUP(F4,$A$16:$B$28,2)*0.01</f>
+        <v>0.13300000000000001</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I10" si="1">B4</f>
-        <v>5.7000000000000002E-3</v>
+        <f t="shared" ref="I4:I10" si="3">VLOOKUP(F4,$A$3:$C$11,2)</f>
+        <v>2.18E-2</v>
       </c>
       <c r="J4" s="7">
-        <f>$N$2*H4</f>
-        <v>30000</v>
+        <f t="shared" si="1"/>
+        <v>13300</v>
       </c>
       <c r="K4" s="6">
-        <f>I4*J4</f>
-        <v>171</v>
+        <f t="shared" ref="K4:K10" si="4">I4*J4</f>
+        <v>289.94</v>
       </c>
       <c r="L4" s="8">
         <f>(K4-K3)/J3</f>
-        <v>5.7000000000000002E-3</v>
+        <v>1.52645697758496E-2</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
+      <c r="A5" s="2">
+        <v>2006</v>
       </c>
       <c r="B5">
         <v>2.18E-2</v>
@@ -952,36 +838,37 @@
       <c r="C5">
         <v>2.9399999999999999E-2</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="F5" s="1">
+        <v>2007</v>
+      </c>
+      <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="H5" s="13">
-        <v>0.3</v>
+        <v>0.85220000000000007</v>
+      </c>
+      <c r="H5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.14779999999999999</v>
       </c>
       <c r="I5" s="4">
+        <f t="shared" si="3"/>
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="J5" s="7">
         <f t="shared" si="1"/>
-        <v>2.18E-2</v>
-      </c>
-      <c r="J5" s="7">
-        <f>$N$2*H5</f>
-        <v>30000</v>
+        <v>14779.999999999998</v>
       </c>
       <c r="K5" s="6">
-        <f t="shared" ref="K4:K11" si="2">I5*J5</f>
-        <v>654</v>
+        <f t="shared" si="4"/>
+        <v>703.52800000000002</v>
       </c>
       <c r="L5" s="8">
-        <f t="shared" ref="L5:L10" si="3">(K5-K4)/J4</f>
-        <v>1.61E-2</v>
+        <f t="shared" ref="L4:L9" si="5">(K5-K4)/J4</f>
+        <v>3.1096842105263159E-2</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
+      <c r="A6" s="1">
+        <v>2007</v>
       </c>
       <c r="B6" s="3">
         <v>4.7600000000000003E-2</v>
@@ -989,36 +876,37 @@
       <c r="C6">
         <v>6.4299999999999996E-2</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="13">
+      <c r="F6" s="2">
+        <v>2008</v>
+      </c>
+      <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="H6" s="13">
-        <v>0.3</v>
+        <v>0.8548</v>
+      </c>
+      <c r="H6" s="16">
+        <f t="shared" si="2"/>
+        <v>0.1452</v>
       </c>
       <c r="I6" s="4">
+        <f t="shared" si="3"/>
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="J6" s="7">
         <f t="shared" si="1"/>
-        <v>4.7600000000000003E-2</v>
-      </c>
-      <c r="J6" s="7">
-        <f>$N$2*H6</f>
-        <v>30000</v>
+        <v>14520</v>
       </c>
       <c r="K6" s="6">
-        <f t="shared" si="2"/>
-        <v>1428</v>
+        <f t="shared" si="4"/>
+        <v>1190.6400000000001</v>
       </c>
       <c r="L6" s="8">
-        <f t="shared" si="3"/>
-        <v>2.58E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.295751014884981E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
+      <c r="A7" s="2">
+        <v>2008</v>
       </c>
       <c r="B7">
         <v>8.2000000000000003E-2</v>
@@ -1026,36 +914,37 @@
       <c r="C7">
         <v>0.1108</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="F7" s="1">
+        <v>2009</v>
+      </c>
+      <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0.3</v>
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="H7" s="16">
+        <f t="shared" si="2"/>
+        <v>0.17300000000000001</v>
       </c>
       <c r="I7" s="4">
-        <f>B7</f>
-        <v>8.2000000000000003E-2</v>
+        <f t="shared" si="3"/>
+        <v>0.1152</v>
       </c>
       <c r="J7" s="7">
-        <f>$N$2*H7</f>
-        <v>30000</v>
+        <f t="shared" si="1"/>
+        <v>17300</v>
       </c>
       <c r="K7" s="6">
-        <f t="shared" si="2"/>
-        <v>2460</v>
+        <f t="shared" si="4"/>
+        <v>1992.96</v>
       </c>
       <c r="L7" s="8">
-        <f t="shared" si="3"/>
-        <v>3.44E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.5256198347107433E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
+      <c r="A8" s="1">
+        <v>2009</v>
       </c>
       <c r="B8">
         <v>0.1152</v>
@@ -1063,36 +952,37 @@
       <c r="C8">
         <v>0.15570000000000001</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="13">
+      <c r="F8" s="2">
+        <v>2010</v>
+      </c>
+      <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="H8" s="13">
-        <v>0.3</v>
+        <v>0.83389999999999997</v>
+      </c>
+      <c r="H8" s="16">
+        <f t="shared" si="2"/>
+        <v>0.1661</v>
       </c>
       <c r="I8" s="4">
+        <f t="shared" si="3"/>
+        <v>0.1416</v>
+      </c>
+      <c r="J8" s="7">
         <f t="shared" si="1"/>
-        <v>0.1152</v>
-      </c>
-      <c r="J8" s="7">
-        <f>$N$2*H8</f>
-        <v>30000</v>
+        <v>16610</v>
       </c>
       <c r="K8" s="6">
-        <f t="shared" si="2"/>
-        <v>3456</v>
+        <f t="shared" si="4"/>
+        <v>2351.9760000000001</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" si="3"/>
-        <v>3.32E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.0752369942196536E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
+      <c r="A9" s="2">
+        <v>2010</v>
       </c>
       <c r="B9">
         <v>0.1416</v>
@@ -1100,36 +990,37 @@
       <c r="C9">
         <v>0.1913</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="13">
+      <c r="F9" s="1">
+        <v>2011</v>
+      </c>
+      <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0.3</v>
+        <v>0.83129999999999993</v>
+      </c>
+      <c r="H9" s="16">
+        <f t="shared" si="2"/>
+        <v>0.16870000000000002</v>
       </c>
       <c r="I9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>0.1416</v>
-      </c>
-      <c r="J9" s="7">
-        <f>$N$2*H9</f>
-        <v>30000</v>
+        <v>16870</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" si="2"/>
-        <v>4248</v>
+        <f t="shared" si="4"/>
+        <v>2969.12</v>
       </c>
       <c r="L9" s="8">
-        <f t="shared" si="3"/>
-        <v>2.64E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.7154966887417207E-2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
+      <c r="A10" s="1">
+        <v>2011</v>
       </c>
       <c r="B10">
         <v>0.17599999999999999</v>
@@ -1137,36 +1028,37 @@
       <c r="C10">
         <v>0.23780000000000001</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="13">
+      <c r="F10" s="2">
+        <v>2017</v>
+      </c>
+      <c r="G10" s="16">
         <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0.3</v>
+        <v>0.79830000000000001</v>
+      </c>
+      <c r="H10" s="16">
+        <f t="shared" si="2"/>
+        <v>0.20170000000000002</v>
       </c>
       <c r="I10" s="4">
+        <f t="shared" si="3"/>
+        <v>0.44209999999999999</v>
+      </c>
+      <c r="J10" s="7">
         <f t="shared" si="1"/>
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="J10" s="7">
-        <f>$N$2*H10</f>
-        <v>30000</v>
+        <v>20170</v>
       </c>
       <c r="K10" s="6">
-        <f t="shared" si="2"/>
-        <v>5280</v>
+        <f t="shared" si="4"/>
+        <v>8917.1569999999992</v>
       </c>
       <c r="L10" s="8">
-        <f t="shared" si="3"/>
-        <v>3.44E-2</v>
+        <f>(K10-K9)/J9</f>
+        <v>0.35258073503260223</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
+      <c r="A11" s="2">
+        <v>2017</v>
       </c>
       <c r="B11">
         <v>0.44209999999999999</v>
@@ -1174,71 +1066,47 @@
       <c r="C11">
         <v>0.59750000000000003</v>
       </c>
-      <c r="F11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="13">
-        <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="H11" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="I11" s="4">
-        <f>B11</f>
-        <v>0.44209999999999999</v>
-      </c>
-      <c r="J11" s="7">
-        <f>$N$2*H11</f>
-        <v>30000</v>
-      </c>
-      <c r="K11" s="6">
-        <f t="shared" si="2"/>
-        <v>13263</v>
-      </c>
-      <c r="L11" s="8">
-        <f>(K11-K10)/J10</f>
-        <v>0.2661</v>
-      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="N13" t="s">
-        <v>21</v>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="str">
+        <f>G1</f>
+        <v>HIV -</v>
+      </c>
+      <c r="H13" t="str">
+        <f>H1</f>
+        <v>HIV Prevalence</v>
+      </c>
+      <c r="I13" t="str">
+        <f>I1</f>
+        <v>ART</v>
+      </c>
+      <c r="J13" t="str">
+        <f>J1</f>
+        <v xml:space="preserve">Number of population (HIV +) </v>
+      </c>
+      <c r="K13" t="str">
+        <f>K1</f>
+        <v xml:space="preserve">Number of population (ART) </v>
+      </c>
+      <c r="L13" t="str">
+        <f>L1</f>
+        <v>ART rate initiation (eta_3,4)</v>
+      </c>
+      <c r="N13" s="9">
+        <v>100000</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" ref="F14:L23" si="4">G1</f>
-        <v>HIV -</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="4"/>
-        <v>HIV Prevalence</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="4"/>
-        <v>ART</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">Number of population (HIV +) </v>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">Number of population (ART) </v>
-      </c>
-      <c r="L14" t="str">
-        <f t="shared" si="4"/>
-        <v>ART rate initiation (eta_3,4)</v>
-      </c>
-      <c r="N14" s="9">
-        <v>100000</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -1251,338 +1119,389 @@
       <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F15" s="17">
+        <f>F3</f>
+        <v>2005</v>
+      </c>
+      <c r="G15" s="16">
+        <f t="shared" ref="G15:G21" si="6">1-H15</f>
+        <v>0.74509999999999998</v>
+      </c>
+      <c r="H15" s="16">
+        <f>VLOOKUP(F15,$A$15:$C$28,3)*0.01</f>
+        <v>0.25490000000000002</v>
+      </c>
+      <c r="I15" s="4">
+        <f>VLOOKUP(F15,$A$3:$C$11,3)</f>
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" ref="J15:J21" si="7">$N$13*H15</f>
+        <v>25490</v>
+      </c>
+      <c r="K15" s="10">
+        <f>K3</f>
+        <v>78.831000000000003</v>
+      </c>
+      <c r="L15" s="8">
+        <f>(K15-0)/J15</f>
+        <v>3.0926245586504514E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>2004</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="F16" t="str">
-        <f t="shared" si="4"/>
-        <v>2004 </v>
-      </c>
-      <c r="G16" s="13">
-        <f>1-H16</f>
-        <v>0.7</v>
-      </c>
-      <c r="H16" s="13">
-        <f>0.3</f>
-        <v>0.3</v>
-      </c>
-      <c r="I16">
-        <f>C3</f>
-        <v>0</v>
+        <v>2005</v>
+      </c>
+      <c r="B16">
+        <v>13.83</v>
+      </c>
+      <c r="C16">
+        <v>25.49</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="F16" s="17">
+        <f>F4</f>
+        <v>2006</v>
+      </c>
+      <c r="G16" s="16">
+        <f t="shared" si="6"/>
+        <v>0.74790000000000001</v>
+      </c>
+      <c r="H16" s="16">
+        <f t="shared" ref="H16:H22" si="8">VLOOKUP(F16,$A$15:$C$28,3)*0.01</f>
+        <v>0.25209999999999999</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" ref="I16:I22" si="9">VLOOKUP(F16,$A$3:$C$11,3)</f>
+        <v>2.9399999999999999E-2</v>
       </c>
       <c r="J16" s="7">
-        <f>$N$14*H16</f>
-        <v>30000</v>
+        <f t="shared" si="7"/>
+        <v>25210</v>
       </c>
       <c r="K16" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>K4</f>
+        <v>289.94</v>
+      </c>
+      <c r="L16" s="8">
+        <f>(K16-K15)/J15</f>
+        <v>8.2820321694782265E-3</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>2005</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="F17" t="str">
-        <f t="shared" si="4"/>
-        <v>2005 </v>
-      </c>
-      <c r="G17" s="13">
-        <f t="shared" ref="G17:G25" si="5">1-H17</f>
-        <v>0.7</v>
-      </c>
-      <c r="H17" s="13">
-        <f t="shared" ref="H17:H25" si="6">0.3</f>
-        <v>0.3</v>
-      </c>
-      <c r="I17">
-        <f t="shared" ref="I17:I23" si="7">C4</f>
-        <v>7.7000000000000002E-3</v>
+      <c r="A17" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B17">
+        <v>13.3</v>
+      </c>
+      <c r="C17">
+        <v>25.21</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="F17" s="17">
+        <f>F5</f>
+        <v>2007</v>
+      </c>
+      <c r="G17" s="16">
+        <f t="shared" si="6"/>
+        <v>0.72589999999999999</v>
+      </c>
+      <c r="H17" s="16">
+        <f t="shared" si="8"/>
+        <v>0.27410000000000001</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="9"/>
+        <v>6.4299999999999996E-2</v>
       </c>
       <c r="J17" s="7">
-        <f t="shared" ref="J17:J25" si="8">$N$14*H17</f>
-        <v>30000</v>
-      </c>
-      <c r="K17" s="10">
-        <f t="shared" si="4"/>
-        <v>171</v>
-      </c>
-      <c r="L17" s="11">
-        <f>L4</f>
-        <v>5.7000000000000002E-3</v>
+        <f t="shared" si="7"/>
+        <v>27410</v>
+      </c>
+      <c r="K17" s="11">
+        <f>K5</f>
+        <v>703.52800000000002</v>
+      </c>
+      <c r="L17" s="8">
+        <f t="shared" ref="L17:L22" si="10">(K17-K16)/J16</f>
+        <v>1.6405712019040064E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>2006</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="4"/>
-        <v>2006 </v>
-      </c>
-      <c r="G18" s="13">
-        <f t="shared" si="5"/>
-        <v>0.7</v>
-      </c>
-      <c r="H18" s="13">
+        <v>2007</v>
+      </c>
+      <c r="B18">
+        <v>14.78</v>
+      </c>
+      <c r="C18">
+        <v>27.41</v>
+      </c>
+      <c r="F18" s="17">
+        <f>F6</f>
+        <v>2008</v>
+      </c>
+      <c r="G18" s="16">
         <f t="shared" si="6"/>
-        <v>0.3</v>
-      </c>
-      <c r="I18">
+        <v>0.71100000000000008</v>
+      </c>
+      <c r="H18" s="16">
+        <f t="shared" si="8"/>
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="9"/>
+        <v>0.1108</v>
+      </c>
+      <c r="J18" s="7">
         <f t="shared" si="7"/>
-        <v>2.9399999999999999E-2</v>
-      </c>
-      <c r="J18" s="7">
+        <v>28899.999999999996</v>
+      </c>
+      <c r="K18" s="10">
+        <f>K6</f>
+        <v>1190.6400000000001</v>
+      </c>
+      <c r="L18" s="8">
+        <f t="shared" si="10"/>
+        <v>1.7771324334184609E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B19">
+        <v>14.52</v>
+      </c>
+      <c r="C19">
+        <v>28.9</v>
+      </c>
+      <c r="F19" s="17">
+        <f>F7</f>
+        <v>2009</v>
+      </c>
+      <c r="G19" s="16">
+        <f t="shared" si="6"/>
+        <v>0.68280000000000007</v>
+      </c>
+      <c r="H19" s="16">
         <f t="shared" si="8"/>
-        <v>30000</v>
-      </c>
-      <c r="K18" s="10">
-        <f t="shared" si="4"/>
-        <v>654</v>
-      </c>
-      <c r="L18" s="10">
-        <f t="shared" si="4"/>
-        <v>1.61E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="F19" t="str">
-        <f t="shared" si="4"/>
-        <v>2007 </v>
-      </c>
-      <c r="G19" s="13">
-        <f t="shared" si="5"/>
-        <v>0.7</v>
-      </c>
-      <c r="H19" s="13">
-        <f t="shared" si="6"/>
-        <v>0.3</v>
-      </c>
-      <c r="I19">
+        <v>0.31719999999999998</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="9"/>
+        <v>0.15570000000000001</v>
+      </c>
+      <c r="J19" s="7">
         <f t="shared" si="7"/>
-        <v>6.4299999999999996E-2</v>
-      </c>
-      <c r="J19" s="7">
-        <f t="shared" si="8"/>
-        <v>30000</v>
-      </c>
-      <c r="K19" s="12">
-        <f>K6</f>
-        <v>1428</v>
-      </c>
-      <c r="L19" s="10">
-        <f t="shared" si="4"/>
-        <v>2.58E-2</v>
+        <v>31720</v>
+      </c>
+      <c r="K19" s="10">
+        <f>K7</f>
+        <v>1992.96</v>
+      </c>
+      <c r="L19" s="8">
+        <f t="shared" si="10"/>
+        <v>2.7761937716262976E-2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>2008</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="F20" t="str">
-        <f t="shared" si="4"/>
-        <v>2008 </v>
-      </c>
-      <c r="G20" s="13">
-        <f t="shared" si="5"/>
-        <v>0.7</v>
-      </c>
-      <c r="H20" s="13">
+        <v>2009</v>
+      </c>
+      <c r="B20">
+        <v>17.3</v>
+      </c>
+      <c r="C20">
+        <v>31.72</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="F20" s="17">
+        <f>F8</f>
+        <v>2010</v>
+      </c>
+      <c r="G20" s="16">
         <f t="shared" si="6"/>
-        <v>0.3</v>
-      </c>
-      <c r="I20">
-        <f>C7</f>
-        <v>0.1108</v>
+        <v>0.65290000000000004</v>
+      </c>
+      <c r="H20" s="16">
+        <f t="shared" si="8"/>
+        <v>0.34710000000000002</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="9"/>
+        <v>0.1913</v>
       </c>
       <c r="J20" s="7">
+        <f t="shared" si="7"/>
+        <v>34710</v>
+      </c>
+      <c r="K20" s="10">
+        <f>K8</f>
+        <v>2351.9760000000001</v>
+      </c>
+      <c r="L20" s="8">
+        <f t="shared" si="10"/>
+        <v>1.1318284993694833E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B21">
+        <v>16.61</v>
+      </c>
+      <c r="C21">
+        <v>34.71</v>
+      </c>
+      <c r="F21" s="17">
+        <f>F9</f>
+        <v>2011</v>
+      </c>
+      <c r="G21" s="16">
+        <f t="shared" si="6"/>
+        <v>0.64860000000000007</v>
+      </c>
+      <c r="H21" s="16">
         <f t="shared" si="8"/>
-        <v>30000</v>
-      </c>
-      <c r="K20" s="10">
-        <f t="shared" si="4"/>
-        <v>2460</v>
-      </c>
-      <c r="L20" s="10">
-        <f t="shared" si="4"/>
-        <v>3.44E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>2009</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="4"/>
-        <v>2009 </v>
-      </c>
-      <c r="G21" s="13">
-        <f t="shared" si="5"/>
-        <v>0.7</v>
-      </c>
-      <c r="H21" s="13">
-        <f t="shared" si="6"/>
-        <v>0.3</v>
-      </c>
-      <c r="I21">
+        <v>0.35139999999999999</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="9"/>
+        <v>0.23780000000000001</v>
+      </c>
+      <c r="J21" s="7">
         <f t="shared" si="7"/>
-        <v>0.15570000000000001</v>
-      </c>
-      <c r="J21" s="7">
-        <f t="shared" si="8"/>
-        <v>30000</v>
+        <v>35140</v>
       </c>
       <c r="K21" s="10">
-        <f t="shared" si="4"/>
-        <v>3456</v>
-      </c>
-      <c r="L21" s="10">
-        <f t="shared" si="4"/>
-        <v>3.32E-2</v>
+        <f>K9</f>
+        <v>2969.12</v>
+      </c>
+      <c r="L21" s="8">
+        <f t="shared" si="10"/>
+        <v>1.7780005762028227E-2</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>2010</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="4"/>
-        <v>2010 </v>
-      </c>
-      <c r="G22" s="13">
-        <f t="shared" si="5"/>
-        <v>0.7</v>
-      </c>
-      <c r="H22" s="13">
-        <f t="shared" si="6"/>
-        <v>0.3</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="7"/>
-        <v>0.1913</v>
+        <v>2011</v>
+      </c>
+      <c r="B22">
+        <v>16.87</v>
+      </c>
+      <c r="C22">
+        <v>35.14</v>
+      </c>
+      <c r="F22" s="17">
+        <f>F10</f>
+        <v>2017</v>
+      </c>
+      <c r="G22" s="16">
+        <f>1-H22</f>
+        <v>0.59549999999999992</v>
+      </c>
+      <c r="H22" s="16">
+        <f t="shared" si="8"/>
+        <v>0.40450000000000003</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="9"/>
+        <v>0.59750000000000003</v>
       </c>
       <c r="J22" s="7">
-        <f t="shared" si="8"/>
-        <v>30000</v>
+        <f>$N$13*H22</f>
+        <v>40450</v>
       </c>
       <c r="K22" s="10">
-        <f t="shared" si="4"/>
-        <v>4248</v>
-      </c>
-      <c r="L22" s="10">
-        <f t="shared" si="4"/>
-        <v>2.64E-2</v>
+        <f>K10</f>
+        <v>8917.1569999999992</v>
+      </c>
+      <c r="L22" s="8">
+        <f>(K22-K21)/J21</f>
+        <v>0.16926684689812177</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>2011</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="4"/>
-        <v>2011 </v>
-      </c>
-      <c r="G23" s="13">
-        <f t="shared" si="5"/>
-        <v>0.7</v>
-      </c>
-      <c r="H23" s="13">
-        <f t="shared" si="6"/>
-        <v>0.3</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="7"/>
-        <v>0.23780000000000001</v>
-      </c>
-      <c r="J23" s="7">
-        <f t="shared" si="8"/>
-        <v>30000</v>
-      </c>
-      <c r="K23" s="10">
-        <f t="shared" si="4"/>
-        <v>5280</v>
-      </c>
-      <c r="L23" s="10">
-        <f t="shared" si="4"/>
-        <v>3.44E-2</v>
+      <c r="A23" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B23">
+        <v>17.48</v>
+      </c>
+      <c r="C23">
+        <v>36.19</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>2012</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" t="str">
-        <f>F11</f>
-        <v>2017 </v>
-      </c>
-      <c r="G24" s="13">
-        <f>1-H24</f>
-        <v>0.7</v>
-      </c>
-      <c r="H24" s="13">
-        <f t="shared" si="6"/>
-        <v>0.3</v>
-      </c>
-      <c r="I24">
-        <f>C11</f>
-        <v>0.59750000000000003</v>
-      </c>
-      <c r="J24" s="7">
-        <f>$N$14*H24</f>
-        <v>30000</v>
-      </c>
-      <c r="K24" s="10">
-        <f>K11</f>
-        <v>13263</v>
-      </c>
-      <c r="L24" s="10">
-        <f>L11</f>
-        <v>0.2661</v>
-      </c>
+      <c r="A24" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B24">
+        <v>19.13</v>
+      </c>
+      <c r="C24">
+        <v>38.119999999999997</v>
+      </c>
+      <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B25">
+        <v>20.87</v>
+      </c>
+      <c r="C25">
+        <v>40.76</v>
+      </c>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B26">
+        <v>18.96</v>
+      </c>
+      <c r="C26">
+        <v>41.81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B27">
+        <v>19.91</v>
+      </c>
+      <c r="C27">
+        <v>42.06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
         <v>2017</v>
       </c>
-      <c r="B25">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="C25">
-        <v>0.26300000000000001</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H29" t="s">
-        <v>79</v>
-      </c>
+      <c r="B28">
+        <v>20.170000000000002</v>
+      </c>
+      <c r="C28">
+        <v>40.450000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="14"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="14"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="15"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D25" r:id="rId1" xr:uid="{7FF81E16-A9C4-6F48-9D52-219843D03B84}"/>
-    <hyperlink ref="D24" r:id="rId2" xr:uid="{5EE437B9-D6FA-604C-9510-6127131DD1A4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1599,7 +1518,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B1">
         <v>2002</v>
@@ -1616,60 +1535,60 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="15">
+        <v>18</v>
+      </c>
+      <c r="C2" s="13">
         <v>0.95</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="15">
+        <v>18</v>
+      </c>
+      <c r="G2" s="13">
         <v>0.95</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="15">
+        <v>18</v>
+      </c>
+      <c r="K2" s="13">
         <v>0.95</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="15">
+        <v>18</v>
+      </c>
+      <c r="O2" s="13">
         <v>0.95</v>
       </c>
       <c r="P2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1681,7 +1600,7 @@
         <v>10.7</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1693,7 +1612,7 @@
         <v>1.9</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -1705,7 +1624,7 @@
         <v>3.8</v>
       </c>
       <c r="N3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="O3">
         <v>3</v>
@@ -1717,15 +1636,15 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="R3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1737,7 +1656,7 @@
         <v>6.6</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -1749,7 +1668,7 @@
         <v>8.9</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1761,7 +1680,7 @@
         <v>9</v>
       </c>
       <c r="N4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="O4">
         <v>3</v>
@@ -1773,15 +1692,15 @@
         <v>12.2</v>
       </c>
       <c r="R4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>694</v>
@@ -1790,7 +1709,7 @@
         <v>8.4</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1802,7 +1721,7 @@
         <v>5.4</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1814,7 +1733,7 @@
         <v>5.9</v>
       </c>
       <c r="M5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -1826,15 +1745,15 @@
         <v>7.8</v>
       </c>
       <c r="Q5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C6">
         <v>540</v>
@@ -1843,7 +1762,7 @@
         <v>14.9</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1855,7 +1774,7 @@
         <v>12.6</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="J6">
         <v>960</v>
@@ -1864,7 +1783,7 @@
         <v>12.6</v>
       </c>
       <c r="L6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -1876,12 +1795,12 @@
         <v>14.7</v>
       </c>
       <c r="P6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1893,7 +1812,7 @@
         <v>11.7</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -1905,7 +1824,7 @@
         <v>16.5</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -1917,7 +1836,7 @@
         <v>15.8</v>
       </c>
       <c r="M7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="N7">
         <v>6</v>
@@ -1929,15 +1848,15 @@
         <v>17.399999999999999</v>
       </c>
       <c r="Q7" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C8">
         <v>626</v>
@@ -1946,7 +1865,7 @@
         <v>10.3</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1958,7 +1877,7 @@
         <v>10.9</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1970,7 +1889,7 @@
         <v>11.3</v>
       </c>
       <c r="M8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1982,12 +1901,12 @@
         <v>13.9</v>
       </c>
       <c r="Q8" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1999,7 +1918,7 @@
         <v>14.7</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -2011,7 +1930,7 @@
         <v>10.8</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -2023,7 +1942,7 @@
         <v>10.3</v>
       </c>
       <c r="M9" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="N9">
         <v>2</v>
@@ -2035,12 +1954,12 @@
         <v>12.8</v>
       </c>
       <c r="Q9" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B10">
         <v>550</v>
@@ -2049,7 +1968,7 @@
         <v>14.1</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2061,7 +1980,7 @@
         <v>15.2</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="I10">
         <v>988</v>
@@ -2070,7 +1989,7 @@
         <v>15.4</v>
       </c>
       <c r="K10" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -2082,12 +2001,12 @@
         <v>14.5</v>
       </c>
       <c r="O10" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B11">
         <v>679</v>
@@ -2096,7 +2015,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -2108,7 +2027,7 @@
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -2120,7 +2039,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="L11" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="M11">
         <v>2</v>
@@ -2132,12 +2051,12 @@
         <v>9.4</v>
       </c>
       <c r="P11" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add HIV incidence to ART_initiation_rate sheet
</commit_message>
<xml_diff>
--- a/param_files/ART_initiation_rate.xlsx
+++ b/param_files/ART_initiation_rate.xlsx
@@ -1,33 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/ws/github/epi_model_HIV_TB/param_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/param_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66331EF-2973-034D-A210-D49F86B1E59A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D29D43A-A8D5-A94C-BF02-27EDD4C518AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="1000" windowWidth="20340" windowHeight="16480" activeTab="1" xr2:uid="{23E87AAA-F98F-6E44-8E92-6D3127C9E120}"/>
+    <workbookView xWindow="4800" yWindow="4340" windowWidth="20340" windowHeight="16480" xr2:uid="{23E87AAA-F98F-6E44-8E92-6D3127C9E120}"/>
   </bookViews>
   <sheets>
-    <sheet name="raw data" sheetId="1" r:id="rId1"/>
+    <sheet name="art_initiation_rate" sheetId="1" r:id="rId1"/>
     <sheet name="linearized" sheetId="3" r:id="rId2"/>
     <sheet name="eta_2,3" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="35">
   <si>
     <r>
       <t>ART coverage over time by gender</t>
@@ -55,16 +64,10 @@
     <t>HIV -</t>
   </si>
   <si>
-    <t>ART</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of population (HIV +) </t>
   </si>
   <si>
     <t xml:space="preserve">Number of population (ART) </t>
-  </si>
-  <si>
-    <t>ART rate initiation (eta_3,4)</t>
   </si>
   <si>
     <t>FEMALES</t>
@@ -108,9 +111,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Population eligible but not on ART</t>
-  </si>
-  <si>
     <t>per year (linearlized)</t>
   </si>
   <si>
@@ -120,12 +120,6 @@
     <t xml:space="preserve">Number of population (HIV -) </t>
   </si>
   <si>
-    <t>Proportion from 2 in HIV</t>
-  </si>
-  <si>
-    <t>Proportion from 3 in HIV</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -148,20 +142,42 @@
   </si>
   <si>
     <t>after July, 2011, ≤350 cells per μL for all individuals</t>
+  </si>
+  <si>
+    <t>ART rate initiation</t>
+  </si>
+  <si>
+    <t>Proportion from CD4 &gt;=200</t>
+  </si>
+  <si>
+    <t>Proportion from CD4 &lt; 200</t>
+  </si>
+  <si>
+    <t>ART coverage over time by gender </t>
+  </si>
+  <si>
+    <t>Population HIV+ but not on ART</t>
+  </si>
+  <si>
+    <t>Incidence Rate</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;????_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,8 +262,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,7 +286,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,7 +312,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -298,19 +334,30 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -630,54 +677,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD3C5C0-7259-F74C-B74F-4B62E66F4BA2}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
     <col min="11" max="11" width="15.83203125" customWidth="1"/>
     <col min="12" max="13" width="17.5" customWidth="1"/>
     <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="51">
+    <row r="1" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -691,7 +739,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2004</v>
       </c>
@@ -716,25 +764,25 @@
         <f>VLOOKUP(F3,$A$3:$C$11,2)</f>
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="J3" s="27">
+      <c r="J3" s="22">
         <f>$P$2-K3</f>
         <v>86170</v>
       </c>
       <c r="K3" s="7">
-        <f t="shared" ref="K3:K10" si="1">$P$2*H3</f>
+        <f>$P$2*H3</f>
         <v>13830</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="21">
         <f>I3*K3</f>
         <v>78.831000000000003</v>
       </c>
-      <c r="M3" s="25">
+      <c r="M3" s="21">
         <f>K3-L3</f>
         <v>13751.169</v>
       </c>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2005</v>
       </c>
@@ -756,31 +804,32 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I10" si="2">VLOOKUP(F4,$A$3:$C$11,2)</f>
+        <f t="shared" ref="I4:I10" si="1">VLOOKUP(F4,$A$3:$C$11,2)</f>
         <v>2.18E-2</v>
       </c>
-      <c r="J4" s="27">
-        <f t="shared" ref="J4:J10" si="3">$P$2-K4</f>
+      <c r="J4" s="22">
+        <f t="shared" ref="J4:J10" si="2">$P$2-K4</f>
         <v>86700</v>
       </c>
       <c r="K4" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K3:K10" si="3">$P$2*H4</f>
         <v>13300</v>
       </c>
-      <c r="L4" s="25">
-        <f t="shared" ref="L4:L10" si="4">I4*K4</f>
+      <c r="L4" s="21">
+        <f>I4*K4</f>
         <v>289.94</v>
       </c>
-      <c r="M4" s="25">
-        <f t="shared" ref="M4:M10" si="5">K4-L4</f>
+      <c r="M4" s="21">
+        <f>K4-L4</f>
         <v>13010.06</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="34">
         <f>(L4-L3)/M3</f>
         <v>1.5352076612541085E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="O4" s="23"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2006</v>
       </c>
@@ -798,35 +847,36 @@
         <v>0.85220000000000007</v>
       </c>
       <c r="H5" s="14">
-        <f t="shared" ref="H5:H10" si="6">VLOOKUP(F5,$A$16:$B$28,2)*0.01</f>
+        <f>VLOOKUP(F5,$A$16:$B$28,2)*0.01</f>
         <v>0.14779999999999999</v>
       </c>
       <c r="I5" s="4">
+        <f t="shared" si="1"/>
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="J5" s="22">
         <f t="shared" si="2"/>
-        <v>4.7600000000000003E-2</v>
-      </c>
-      <c r="J5" s="27">
+        <v>85220</v>
+      </c>
+      <c r="K5" s="7">
         <f t="shared" si="3"/>
-        <v>85220</v>
-      </c>
-      <c r="K5" s="7">
-        <f t="shared" si="1"/>
         <v>14779.999999999998</v>
       </c>
-      <c r="L5" s="25">
-        <f t="shared" si="4"/>
+      <c r="L5" s="21">
+        <f t="shared" ref="L4:L10" si="4">I5*K5</f>
         <v>703.52800000000002</v>
       </c>
-      <c r="M5" s="25">
-        <f t="shared" si="5"/>
+      <c r="M5" s="21">
+        <f t="shared" ref="M4:M10" si="5">K5-L5</f>
         <v>14076.471999999998</v>
       </c>
-      <c r="N5" s="8">
-        <f t="shared" ref="N5:N10" si="7">(L5-L4)/M4</f>
+      <c r="N5" s="34">
+        <f t="shared" ref="N5:N10" si="6">(L5-L4)/M4</f>
         <v>3.1789861076736009E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="O5" s="23"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2007</v>
       </c>
@@ -844,35 +894,36 @@
         <v>0.8548</v>
       </c>
       <c r="H6" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H5:H10" si="7">VLOOKUP(F6,$A$16:$B$28,2)*0.01</f>
         <v>0.1452</v>
       </c>
       <c r="I6" s="4">
+        <f t="shared" si="1"/>
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="J6" s="22">
         <f t="shared" si="2"/>
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="J6" s="27">
+        <v>85480</v>
+      </c>
+      <c r="K6" s="7">
         <f t="shared" si="3"/>
-        <v>85480</v>
-      </c>
-      <c r="K6" s="7">
-        <f t="shared" si="1"/>
         <v>14520</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="21">
         <f t="shared" si="4"/>
         <v>1190.6400000000001</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="21">
         <f t="shared" si="5"/>
         <v>13329.36</v>
       </c>
-      <c r="N6" s="8">
-        <f t="shared" si="7"/>
+      <c r="N6" s="34">
+        <f t="shared" si="6"/>
         <v>3.4604693562421046E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="O6" s="23"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2008</v>
       </c>
@@ -890,35 +941,36 @@
         <v>0.82699999999999996</v>
       </c>
       <c r="H7" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.17300000000000001</v>
       </c>
       <c r="I7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.1152</v>
+      </c>
+      <c r="J7" s="22">
         <f t="shared" si="2"/>
-        <v>0.1152</v>
-      </c>
-      <c r="J7" s="27">
+        <v>82700</v>
+      </c>
+      <c r="K7" s="7">
         <f t="shared" si="3"/>
-        <v>82700</v>
-      </c>
-      <c r="K7" s="7">
-        <f t="shared" si="1"/>
         <v>17300</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="21">
         <f t="shared" si="4"/>
         <v>1992.96</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="21">
         <f t="shared" si="5"/>
         <v>15307.04</v>
       </c>
-      <c r="N7" s="8">
-        <f t="shared" si="7"/>
+      <c r="N7" s="34">
+        <f t="shared" si="6"/>
         <v>6.0191937197284787E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="O7" s="23"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2009</v>
       </c>
@@ -936,35 +988,36 @@
         <v>0.83389999999999997</v>
       </c>
       <c r="H8" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.1661</v>
       </c>
       <c r="I8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.1416</v>
+      </c>
+      <c r="J8" s="22">
         <f t="shared" si="2"/>
-        <v>0.1416</v>
-      </c>
-      <c r="J8" s="27">
+        <v>83390</v>
+      </c>
+      <c r="K8" s="7">
         <f t="shared" si="3"/>
-        <v>83390</v>
-      </c>
-      <c r="K8" s="7">
-        <f t="shared" si="1"/>
         <v>16610</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="21">
         <f>I8*K8</f>
         <v>2351.9760000000001</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="21">
         <f t="shared" si="5"/>
         <v>14258.023999999999</v>
       </c>
-      <c r="N8" s="8">
-        <f t="shared" si="7"/>
+      <c r="N8" s="34">
+        <f t="shared" si="6"/>
         <v>2.345430599253677E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="18" customHeight="1">
+      <c r="O8" s="23"/>
+    </row>
+    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2010</v>
       </c>
@@ -982,38 +1035,38 @@
         <v>0.83129999999999993</v>
       </c>
       <c r="H9" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.16870000000000002</v>
       </c>
       <c r="I9" s="4">
+        <f t="shared" si="1"/>
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="J9" s="22">
         <f t="shared" si="2"/>
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="J9" s="27">
+        <v>83130</v>
+      </c>
+      <c r="K9" s="7">
         <f t="shared" si="3"/>
-        <v>83130</v>
-      </c>
-      <c r="K9" s="7">
-        <f t="shared" si="1"/>
         <v>16870</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="21">
         <f t="shared" si="4"/>
         <v>2969.12</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="21">
         <f t="shared" si="5"/>
         <v>13900.880000000001</v>
       </c>
-      <c r="N9" s="8">
-        <f t="shared" si="7"/>
+      <c r="N9" s="34">
+        <f t="shared" si="6"/>
         <v>4.3283978200625822E-2</v>
       </c>
-      <c r="O9" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="O9" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2011</v>
       </c>
@@ -1031,39 +1084,39 @@
         <v>0.79830000000000001</v>
       </c>
       <c r="H10" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.20170000000000002</v>
       </c>
       <c r="I10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.44209999999999999</v>
+      </c>
+      <c r="J10" s="22">
         <f t="shared" si="2"/>
-        <v>0.44209999999999999</v>
-      </c>
-      <c r="J10" s="27">
+        <v>79830</v>
+      </c>
+      <c r="K10" s="7">
         <f t="shared" si="3"/>
-        <v>79830</v>
-      </c>
-      <c r="K10" s="7">
-        <f t="shared" si="1"/>
         <v>20170</v>
       </c>
-      <c r="L10" s="25">
+      <c r="L10" s="21">
         <f t="shared" si="4"/>
         <v>8917.1569999999992</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="21">
         <f t="shared" si="5"/>
         <v>11252.843000000001</v>
       </c>
-      <c r="N10" s="8">
-        <f t="shared" si="7"/>
+      <c r="N10" s="34">
+        <f t="shared" si="6"/>
         <v>0.42788924154442015</v>
       </c>
-      <c r="O10" s="8">
+      <c r="O10" s="34">
         <f>(N10-N9)/(F10-F9)</f>
         <v>6.4100877223965722E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2017</v>
       </c>
@@ -1076,29 +1129,29 @@
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="P12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ref="G13:N13" si="8">G1</f>
         <v>HIV -</v>
       </c>
-      <c r="H13" t="str">
+      <c r="H13" s="5" t="str">
         <f t="shared" si="8"/>
         <v>HIV Prevalence</v>
       </c>
-      <c r="I13" t="str">
+      <c r="I13" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>ART</v>
+        <v>ART coverage over time by gender </v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K13" s="5" t="str">
         <f t="shared" si="8"/>
@@ -1108,21 +1161,23 @@
         <f t="shared" si="8"/>
         <v xml:space="preserve">Number of population (ART) </v>
       </c>
-      <c r="M13" s="5"/>
+      <c r="M13" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="N13" s="5" t="str">
         <f t="shared" si="8"/>
-        <v>ART rate initiation (eta_3,4)</v>
+        <v>ART rate initiation</v>
       </c>
       <c r="P13" s="9">
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1148,7 +1203,7 @@
         <f>VLOOKUP(F15,$A$3:$C$11,3)</f>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="J15" s="27">
+      <c r="J15" s="22">
         <f>$P$13-K15</f>
         <v>74510</v>
       </c>
@@ -1156,17 +1211,17 @@
         <f t="shared" ref="K15:K21" si="11">$P$13*H15</f>
         <v>25490</v>
       </c>
-      <c r="L15" s="24">
+      <c r="L15" s="20">
         <f>I15*K15</f>
         <v>196.273</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="21">
         <f>K15-L15</f>
         <v>25293.726999999999</v>
       </c>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2005</v>
       </c>
@@ -1193,7 +1248,7 @@
         <f t="shared" ref="I16:I22" si="13">VLOOKUP(F16,$A$3:$C$11,3)</f>
         <v>2.9399999999999999E-2</v>
       </c>
-      <c r="J16" s="27">
+      <c r="J16" s="22">
         <f t="shared" ref="J16:J22" si="14">$P$13-K16</f>
         <v>74790</v>
       </c>
@@ -1201,20 +1256,21 @@
         <f t="shared" si="11"/>
         <v>25210</v>
       </c>
-      <c r="L16" s="24">
+      <c r="L16" s="20">
         <f t="shared" ref="L16:L22" si="15">I16*K16</f>
         <v>741.17399999999998</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="21">
         <f t="shared" ref="M16:M22" si="16">K16-L16</f>
         <v>24468.826000000001</v>
       </c>
-      <c r="N16" s="8">
+      <c r="N16" s="34">
         <f>(L16-L15)/M15</f>
         <v>2.1542930387443496E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="O16" s="35"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2006</v>
       </c>
@@ -1241,7 +1297,7 @@
         <f t="shared" si="13"/>
         <v>6.4299999999999996E-2</v>
       </c>
-      <c r="J17" s="27">
+      <c r="J17" s="22">
         <f t="shared" si="14"/>
         <v>72590</v>
       </c>
@@ -1249,20 +1305,21 @@
         <f t="shared" si="11"/>
         <v>27410</v>
       </c>
-      <c r="L17" s="24">
+      <c r="L17" s="20">
         <f t="shared" si="15"/>
         <v>1762.463</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="21">
         <f t="shared" si="16"/>
         <v>25647.537</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="34">
         <f>(L17-L16)/M16</f>
         <v>4.173837355335315E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="O17" s="35"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2007</v>
       </c>
@@ -1288,7 +1345,7 @@
         <f t="shared" si="13"/>
         <v>0.1108</v>
       </c>
-      <c r="J18" s="27">
+      <c r="J18" s="22">
         <f t="shared" si="14"/>
         <v>71100</v>
       </c>
@@ -1296,20 +1353,21 @@
         <f t="shared" si="11"/>
         <v>28899.999999999996</v>
       </c>
-      <c r="L18" s="24">
+      <c r="L18" s="20">
         <f t="shared" si="15"/>
         <v>3202.1199999999994</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="21">
         <f t="shared" si="16"/>
         <v>25697.879999999997</v>
       </c>
-      <c r="N18" s="8">
+      <c r="N18" s="34">
         <f t="shared" ref="N18:N21" si="17">(L18-L17)/M17</f>
         <v>5.6132368577926195E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="O18" s="35"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2008</v>
       </c>
@@ -1335,7 +1393,7 @@
         <f t="shared" si="13"/>
         <v>0.15570000000000001</v>
       </c>
-      <c r="J19" s="27">
+      <c r="J19" s="22">
         <f t="shared" si="14"/>
         <v>68280</v>
       </c>
@@ -1343,20 +1401,21 @@
         <f t="shared" si="11"/>
         <v>31720</v>
       </c>
-      <c r="L19" s="24">
+      <c r="L19" s="20">
         <f t="shared" si="15"/>
         <v>4938.8040000000001</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="21">
         <f t="shared" si="16"/>
         <v>26781.196</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="34">
         <f t="shared" si="17"/>
         <v>6.7580827679170452E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="O19" s="35"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>2009</v>
       </c>
@@ -1383,7 +1442,7 @@
         <f t="shared" si="13"/>
         <v>0.1913</v>
       </c>
-      <c r="J20" s="27">
+      <c r="J20" s="22">
         <f t="shared" si="14"/>
         <v>65290</v>
       </c>
@@ -1391,20 +1450,21 @@
         <f t="shared" si="11"/>
         <v>34710</v>
       </c>
-      <c r="L20" s="24">
+      <c r="L20" s="20">
         <f t="shared" si="15"/>
         <v>6640.0230000000001</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="21">
         <f t="shared" si="16"/>
         <v>28069.976999999999</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="34">
         <f t="shared" si="17"/>
         <v>6.3522891210683802E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="51">
+      <c r="O20" s="35"/>
+    </row>
+    <row r="21" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2010</v>
       </c>
@@ -1430,7 +1490,7 @@
         <f t="shared" si="13"/>
         <v>0.23780000000000001</v>
       </c>
-      <c r="J21" s="27">
+      <c r="J21" s="22">
         <f t="shared" si="14"/>
         <v>64860</v>
       </c>
@@ -1438,23 +1498,23 @@
         <f t="shared" si="11"/>
         <v>35140</v>
       </c>
-      <c r="L21" s="24">
+      <c r="L21" s="20">
         <f t="shared" si="15"/>
         <v>8356.2920000000013</v>
       </c>
-      <c r="M21" s="25">
+      <c r="M21" s="21">
         <f t="shared" si="16"/>
         <v>26783.707999999999</v>
       </c>
-      <c r="N21" s="8">
-        <f t="shared" si="17"/>
+      <c r="N21" s="34">
+        <f>(L21-L20)/M20</f>
         <v>6.1142515364369598E-2</v>
       </c>
-      <c r="O21" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="O21" s="36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>2011</v>
       </c>
@@ -1480,7 +1540,7 @@
         <f t="shared" si="13"/>
         <v>0.59750000000000003</v>
       </c>
-      <c r="J22" s="27">
+      <c r="J22" s="22">
         <f t="shared" si="14"/>
         <v>59550</v>
       </c>
@@ -1488,24 +1548,24 @@
         <f>$P$13*H22</f>
         <v>40450</v>
       </c>
-      <c r="L22" s="24">
+      <c r="L22" s="20">
         <f t="shared" si="15"/>
         <v>24168.875</v>
       </c>
-      <c r="M22" s="25">
+      <c r="M22" s="21">
         <f t="shared" si="16"/>
         <v>16281.125</v>
       </c>
-      <c r="N22" s="8">
+      <c r="N22" s="34">
         <f>(L22-L21)/M21</f>
         <v>0.59038065229803127</v>
       </c>
-      <c r="O22" s="8">
+      <c r="O22" s="34">
         <f>(N22-N21)/(F22-F21)</f>
         <v>8.8206356155610274E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>2012</v>
       </c>
@@ -1524,7 +1584,7 @@
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>2013</v>
       </c>
@@ -1536,7 +1596,7 @@
       </c>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>2014</v>
       </c>
@@ -1548,7 +1608,7 @@
       </c>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>2015</v>
       </c>
@@ -1559,7 +1619,7 @@
         <v>41.81</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>2016</v>
       </c>
@@ -1571,7 +1631,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>2017</v>
       </c>
@@ -1583,51 +1643,51 @@
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" s="11"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F34" s="2"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39" s="12"/>
       <c r="F39" s="13"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F40" s="13"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F41" s="13"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F42" s="13"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F43" s="13"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F44" s="13"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F45" s="13"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F46" s="13"/>
     </row>
   </sheetData>
@@ -1637,481 +1697,1090 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002FC0AB-95B4-5043-8C83-5F226B5D5B91}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1990</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1991</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1992</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1993</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1994</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1995</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1996</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="32"/>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1997</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1998</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1999</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2000</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2001</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2002</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2003</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2004</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2005</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>2006</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="19">
+        <f>VLOOKUP(A18,art_initiation_rate!$F$3:$N$10,9)</f>
+        <v>1.5352076612541085E-2</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>2007</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="19">
+        <f>VLOOKUP(A19,art_initiation_rate!$F$3:$N$10,9)</f>
+        <v>3.1789861076736009E-2</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <v>2008</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="19">
+        <f>VLOOKUP(A20,art_initiation_rate!$F$3:$N$10,9)</f>
+        <v>3.4604693562421046E-2</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="18">
+        <v>2009</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="19">
+        <f>VLOOKUP(A21,art_initiation_rate!$F$3:$N$10,9)</f>
+        <v>6.0191937197284787E-2</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="11">
+        <v>2010</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="19">
+        <f>VLOOKUP(A22,art_initiation_rate!$F$3:$N$10,9)</f>
+        <v>2.345430599253677E-2</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="18">
+        <v>2011</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="19">
+        <f>VLOOKUP(A23,art_initiation_rate!$F$3:$N$10,9)</f>
+        <v>4.3283978200625822E-2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="25">
+        <v>2012</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="32"/>
+      <c r="D24" s="26">
+        <f>art_initiation_rate!$O$10</f>
+        <v>6.4100877223965722E-2</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="15" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A25" s="25">
+        <v>2013</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="32"/>
+      <c r="D25" s="26">
+        <f>art_initiation_rate!$O$10</f>
+        <v>6.4100877223965722E-2</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="27"/>
+    </row>
+    <row r="26" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="25">
+        <v>2014</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="32"/>
+      <c r="D26" s="26">
+        <f>art_initiation_rate!$O$10</f>
+        <v>6.4100877223965722E-2</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="28"/>
+    </row>
+    <row r="27" spans="1:8" s="15" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A27" s="25">
+        <v>2015</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="32"/>
+      <c r="D27" s="26">
+        <f>art_initiation_rate!$O$10</f>
+        <v>6.4100877223965722E-2</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="27"/>
+    </row>
+    <row r="28" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="25">
+        <v>2016</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="32"/>
+      <c r="D28" s="26">
+        <f>art_initiation_rate!$O$10</f>
+        <v>6.4100877223965722E-2</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="28"/>
+    </row>
+    <row r="29" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="29">
+        <v>2017</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="32"/>
+      <c r="D29" s="26">
+        <f>art_initiation_rate!$O$10</f>
+        <v>6.4100877223965722E-2</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="30"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1990</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="32"/>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1991</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1992</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="32"/>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1993</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="32"/>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1994</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="32"/>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1995</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="32"/>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1996</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="32"/>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1997</v>
+      </c>
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="32"/>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1998</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="32"/>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1999</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="32"/>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2000</v>
+      </c>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="32"/>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2001</v>
+      </c>
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="32"/>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2002</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="32"/>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2003</v>
+      </c>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="32"/>
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2004</v>
+      </c>
+      <c r="B44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="32"/>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2005</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="32"/>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="29">
+        <v>2006</v>
+      </c>
+      <c r="B46" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="11">
-        <v>2006</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="21">
-        <f>VLOOKUP(A2,'raw data'!$F$3:$N$10,9)</f>
-        <v>1.5352076612541085E-2</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="18">
+      <c r="C46" s="32"/>
+      <c r="D46" s="31">
+        <f>VLOOKUP(A46,art_initiation_rate!$F$13:$N$22,9)</f>
+        <v>2.1542930387443496E-2</v>
+      </c>
+      <c r="E46" s="15">
+        <v>0</v>
+      </c>
+      <c r="F46" s="15">
+        <v>1</v>
+      </c>
+      <c r="H46" s="28"/>
+    </row>
+    <row r="47" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="25">
         <v>2007</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="21">
-        <f>VLOOKUP(A3,'raw data'!$F$3:$N$10,9)</f>
-        <v>3.1789861076736009E-2</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="11">
+      <c r="B47" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="32"/>
+      <c r="D47" s="31">
+        <f>VLOOKUP(A47,art_initiation_rate!$F$13:$N$22,9)</f>
+        <v>4.173837355335315E-2</v>
+      </c>
+      <c r="E47" s="15">
+        <v>0</v>
+      </c>
+      <c r="F47" s="15">
+        <v>1</v>
+      </c>
+      <c r="H47" s="30"/>
+    </row>
+    <row r="48" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="29">
         <v>2008</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="21">
-        <f>VLOOKUP(A4,'raw data'!$F$3:$N$10,9)</f>
-        <v>3.4604693562421046E-2</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="18">
+      <c r="B48" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="32"/>
+      <c r="D48" s="31">
+        <f>VLOOKUP(A48,art_initiation_rate!$F$13:$N$22,9)</f>
+        <v>5.6132368577926195E-2</v>
+      </c>
+      <c r="E48" s="15">
+        <v>0</v>
+      </c>
+      <c r="F48" s="15">
+        <v>1</v>
+      </c>
+      <c r="H48" s="28"/>
+    </row>
+    <row r="49" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="25">
         <v>2009</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="21">
-        <f>VLOOKUP(A5,'raw data'!$F$3:$N$10,9)</f>
-        <v>6.0191937197284787E-2</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="11">
+      <c r="B49" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="32"/>
+      <c r="D49" s="31">
+        <f>VLOOKUP(A49,art_initiation_rate!$F$13:$N$22,9)</f>
+        <v>6.7580827679170452E-2</v>
+      </c>
+      <c r="E49" s="15">
+        <v>0</v>
+      </c>
+      <c r="F49" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="29">
         <v>2010</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="21">
-        <f>VLOOKUP(A6,'raw data'!$F$3:$N$10,9)</f>
-        <v>2.345430599253677E-2</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="18">
+      <c r="B50" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="32"/>
+      <c r="D50" s="31">
+        <f>VLOOKUP(A50,art_initiation_rate!$F$13:$N$22,9)</f>
+        <v>6.3522891210683802E-2</v>
+      </c>
+      <c r="E50" s="15">
+        <v>0</v>
+      </c>
+      <c r="F50" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="25">
         <v>2011</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="21">
-        <f>VLOOKUP(A7,'raw data'!$F$3:$N$10,9)</f>
-        <v>4.3283978200625822E-2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="20">
+      <c r="B51" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="32"/>
+      <c r="D51" s="31">
+        <f>VLOOKUP(A51,art_initiation_rate!$F$13:$N$22,9)</f>
+        <v>6.1142515364369598E-2</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="25">
         <v>2012</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="22">
-        <f>'raw data'!$O$10</f>
-        <v>6.4100877223965722E-2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="20">
-      <c r="A9" s="20">
+      <c r="B52" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="32"/>
+      <c r="D52" s="26">
+        <f>art_initiation_rate!$O$22</f>
+        <v>8.8206356155610274E-2</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="25">
         <v>2013</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="22">
-        <f>'raw data'!$O$10</f>
-        <v>6.4100877223965722E-2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="28"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="20">
+      <c r="B53" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="32"/>
+      <c r="D53" s="26">
+        <f>art_initiation_rate!$O$22</f>
+        <v>8.8206356155610274E-2</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="25">
         <v>2014</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="22">
-        <f>'raw data'!$O$10</f>
-        <v>6.4100877223965722E-2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" ht="20">
-      <c r="A11" s="20">
+      <c r="B54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="32"/>
+      <c r="D54" s="26">
+        <f>art_initiation_rate!$O$22</f>
+        <v>8.8206356155610274E-2</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="25">
         <v>2015</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="22">
-        <f>'raw data'!$O$10</f>
-        <v>6.4100877223965722E-2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="28"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="20">
+      <c r="B55" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="32"/>
+      <c r="D55" s="26">
+        <f>art_initiation_rate!$O$22</f>
+        <v>8.8206356155610274E-2</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="25">
         <v>2016</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="22">
-        <f>'raw data'!$O$10</f>
-        <v>6.4100877223965722E-2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="26">
+      <c r="B56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" s="32"/>
+      <c r="D56" s="26">
+        <f>art_initiation_rate!$O$22</f>
+        <v>8.8206356155610274E-2</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="29">
         <v>2017</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="22">
-        <f>'raw data'!$O$10</f>
-        <v>6.4100877223965722E-2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="29"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="11">
-        <v>2006</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="23">
-        <f>VLOOKUP(A14,'raw data'!$F$13:$N$22,9)</f>
-        <v>2.1542930387443496E-2</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="18">
-        <v>2007</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="23">
-        <f>VLOOKUP(A15,'raw data'!$F$13:$N$22,9)</f>
-        <v>4.173837355335315E-2</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="G15" s="29"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="11">
-        <v>2008</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="23">
-        <f>VLOOKUP(A16,'raw data'!$F$13:$N$22,9)</f>
-        <v>5.6132368577926195E-2</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="18">
-        <v>2009</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="23">
-        <f>VLOOKUP(A17,'raw data'!$F$13:$N$22,9)</f>
-        <v>6.7580827679170452E-2</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="11">
-        <v>2010</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="23">
-        <f>VLOOKUP(A18,'raw data'!$F$13:$N$22,9)</f>
-        <v>6.3522891210683802E-2</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="18">
-        <v>2011</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="23">
-        <f>VLOOKUP(A19,'raw data'!$F$13:$N$22,9)</f>
-        <v>6.1142515364369598E-2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="20">
-        <v>2012</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="22">
-        <f>'raw data'!$O$22</f>
+      <c r="B57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="32"/>
+      <c r="D57" s="26">
+        <f>art_initiation_rate!$O$22</f>
         <v>8.8206356155610274E-2</v>
       </c>
-      <c r="D20" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="20">
-        <v>2013</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="22">
-        <f>'raw data'!$O$22</f>
-        <v>8.8206356155610274E-2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="20">
-        <v>2014</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="22">
-        <f>'raw data'!$O$22</f>
-        <v>8.8206356155610274E-2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="20">
-        <v>2015</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="22">
-        <f>'raw data'!$O$22</f>
-        <v>8.8206356155610274E-2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="20">
-        <v>2016</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="22">
-        <f>'raw data'!$O$22</f>
-        <v>8.8206356155610274E-2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="26">
-        <v>2017</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="22">
-        <f>'raw data'!$O$22</f>
-        <v>8.8206356155610274E-2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" t="s">
-        <v>25</v>
+      <c r="E57" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2124,14 +2793,14 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1">
         <v>0.25</v>
@@ -2149,9 +2818,9 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>0.25</v>
@@ -2169,26 +2838,26 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <f>SUM(B1:E1)</f>
@@ -2199,9 +2868,9 @@
         <v>0.1295336787564767</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <f>SUM(B2:E2)</f>

</xml_diff>

<commit_message>
update ART initation rate file, and incidence
</commit_message>
<xml_diff>
--- a/param_files/ART_initiation_rate.xlsx
+++ b/param_files/ART_initiation_rate.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/param_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D29D43A-A8D5-A94C-BF02-27EDD4C518AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3415C25-C74F-6B4A-AE3F-3708EB4A5216}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="4340" windowWidth="20340" windowHeight="16480" xr2:uid="{23E87AAA-F98F-6E44-8E92-6D3127C9E120}"/>
+    <workbookView xWindow="4800" yWindow="4220" windowWidth="20340" windowHeight="16480" activeTab="1" xr2:uid="{23E87AAA-F98F-6E44-8E92-6D3127C9E120}"/>
   </bookViews>
   <sheets>
     <sheet name="art_initiation_rate" sheetId="1" r:id="rId1"/>
-    <sheet name="linearized" sheetId="3" r:id="rId2"/>
+    <sheet name="input_data" sheetId="3" r:id="rId2"/>
     <sheet name="eta_2,3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -175,7 +175,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;????_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -340,8 +340,8 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -353,9 +353,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -677,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD3C5C0-7259-F74C-B74F-4B62E66F4BA2}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -812,7 +812,7 @@
         <v>86700</v>
       </c>
       <c r="K4" s="7">
-        <f t="shared" ref="K3:K10" si="3">$P$2*H4</f>
+        <f t="shared" ref="K4:K10" si="3">$P$2*H4</f>
         <v>13300</v>
       </c>
       <c r="L4" s="21">
@@ -863,11 +863,11 @@
         <v>14779.999999999998</v>
       </c>
       <c r="L5" s="21">
-        <f t="shared" ref="L4:L10" si="4">I5*K5</f>
+        <f t="shared" ref="L5:L10" si="4">I5*K5</f>
         <v>703.52800000000002</v>
       </c>
       <c r="M5" s="21">
-        <f t="shared" ref="M4:M10" si="5">K5-L5</f>
+        <f t="shared" ref="M5:M10" si="5">K5-L5</f>
         <v>14076.471999999998</v>
       </c>
       <c r="N5" s="34">
@@ -894,7 +894,7 @@
         <v>0.8548</v>
       </c>
       <c r="H6" s="14">
-        <f t="shared" ref="H5:H10" si="7">VLOOKUP(F6,$A$16:$B$28,2)*0.01</f>
+        <f t="shared" ref="H6:H10" si="7">VLOOKUP(F6,$A$16:$B$28,2)*0.01</f>
         <v>0.1452</v>
       </c>
       <c r="I6" s="4">
@@ -1362,7 +1362,7 @@
         <v>25697.879999999997</v>
       </c>
       <c r="N18" s="34">
-        <f t="shared" ref="N18:N21" si="17">(L18-L17)/M17</f>
+        <f t="shared" ref="N18:N20" si="17">(L18-L17)/M17</f>
         <v>5.6132368577926195E-2</v>
       </c>
       <c r="O18" s="35"/>
@@ -1699,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002FC0AB-95B4-5043-8C83-5F226B5D5B91}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add H IV incidence to ART_initiation_rate sheet
</commit_message>
<xml_diff>
--- a/param_files/ART_initiation_rate.xlsx
+++ b/param_files/ART_initiation_rate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/param_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3415C25-C74F-6B4A-AE3F-3708EB4A5216}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429088F4-22A1-2C4E-AB60-41CBB2B45AE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="4220" windowWidth="20340" windowHeight="16480" activeTab="1" xr2:uid="{23E87AAA-F98F-6E44-8E92-6D3127C9E120}"/>
   </bookViews>
@@ -312,7 +312,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -358,6 +358,7 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -675,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD3C5C0-7259-F74C-B74F-4B62E66F4BA2}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,28 +741,24 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>2004</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
+      <c r="A3" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="F3" s="1">
         <v>2005</v>
       </c>
       <c r="G3" s="14">
-        <f t="shared" ref="G3:G10" si="0">1-H3</f>
+        <f>1-H3</f>
         <v>0.86170000000000002</v>
       </c>
       <c r="H3" s="14">
-        <f>VLOOKUP(F3,$A$16:$B$28,2)*0.01</f>
+        <f>VLOOKUP(F3,$A$46:$B$58,2)*0.01</f>
         <v>0.13830000000000001</v>
       </c>
       <c r="I3" s="4">
-        <f>VLOOKUP(F3,$A$3:$C$11,2)</f>
+        <f>VLOOKUP(F3,$A$18:$C$26,2)</f>
         <v>5.7000000000000002E-3</v>
       </c>
       <c r="J3" s="22">
@@ -784,35 +781,31 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>2005</v>
-      </c>
-      <c r="B4">
-        <v>5.7000000000000002E-3</v>
-      </c>
-      <c r="C4">
-        <v>7.7000000000000002E-3</v>
-      </c>
+        <v>1991</v>
+      </c>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="F4" s="2">
         <v>2006</v>
       </c>
       <c r="G4" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G4:G10" si="0">1-H4</f>
         <v>0.86699999999999999</v>
       </c>
       <c r="H4" s="14">
-        <f>VLOOKUP(F4,$A$16:$B$28,2)*0.01</f>
+        <f>VLOOKUP(F4,$A$46:$B$58,2)*0.01</f>
         <v>0.13300000000000001</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" ref="I4:I10" si="1">VLOOKUP(F4,$A$3:$C$11,2)</f>
+        <f>VLOOKUP(F4,$A$18:$C$26,2)</f>
         <v>2.18E-2</v>
       </c>
       <c r="J4" s="22">
-        <f t="shared" ref="J4:J10" si="2">$P$2-K4</f>
+        <f t="shared" ref="J4:J10" si="1">$P$2-K4</f>
         <v>86700</v>
       </c>
       <c r="K4" s="7">
-        <f t="shared" ref="K4:K10" si="3">$P$2*H4</f>
+        <f t="shared" ref="K4:K10" si="2">$P$2*H4</f>
         <v>13300</v>
       </c>
       <c r="L4" s="21">
@@ -830,15 +823,11 @@
       <c r="O4" s="23"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>2006</v>
-      </c>
-      <c r="B5">
-        <v>2.18E-2</v>
-      </c>
-      <c r="C5">
-        <v>2.9399999999999999E-2</v>
-      </c>
+      <c r="A5" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
       <c r="F5" s="1">
         <v>2007</v>
       </c>
@@ -847,45 +836,41 @@
         <v>0.85220000000000007</v>
       </c>
       <c r="H5" s="14">
-        <f>VLOOKUP(F5,$A$16:$B$28,2)*0.01</f>
+        <f>VLOOKUP(F5,$A$46:$B$58,2)*0.01</f>
         <v>0.14779999999999999</v>
       </c>
       <c r="I5" s="4">
+        <f>VLOOKUP(F5,$A$18:$C$26,2)</f>
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="J5" s="22">
         <f t="shared" si="1"/>
-        <v>4.7600000000000003E-2</v>
-      </c>
-      <c r="J5" s="22">
+        <v>85220</v>
+      </c>
+      <c r="K5" s="7">
         <f t="shared" si="2"/>
-        <v>85220</v>
-      </c>
-      <c r="K5" s="7">
-        <f t="shared" si="3"/>
         <v>14779.999999999998</v>
       </c>
       <c r="L5" s="21">
-        <f t="shared" ref="L5:L10" si="4">I5*K5</f>
+        <f t="shared" ref="L5:L10" si="3">I5*K5</f>
         <v>703.52800000000002</v>
       </c>
       <c r="M5" s="21">
-        <f t="shared" ref="M5:M10" si="5">K5-L5</f>
+        <f t="shared" ref="M5:M10" si="4">K5-L5</f>
         <v>14076.471999999998</v>
       </c>
       <c r="N5" s="34">
-        <f t="shared" ref="N5:N10" si="6">(L5-L4)/M4</f>
+        <f t="shared" ref="N5:N10" si="5">(L5-L4)/M4</f>
         <v>3.1789861076736009E-2</v>
       </c>
       <c r="O5" s="23"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B6" s="3">
-        <v>4.7600000000000003E-2</v>
-      </c>
-      <c r="C6">
-        <v>6.4299999999999996E-2</v>
-      </c>
+        <v>1993</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
       <c r="F6" s="2">
         <v>2008</v>
       </c>
@@ -894,45 +879,41 @@
         <v>0.8548</v>
       </c>
       <c r="H6" s="14">
-        <f t="shared" ref="H6:H10" si="7">VLOOKUP(F6,$A$16:$B$28,2)*0.01</f>
+        <f>VLOOKUP(F6,$A$46:$B$58,2)*0.01</f>
         <v>0.1452</v>
       </c>
       <c r="I6" s="4">
+        <f>VLOOKUP(F6,$A$18:$C$26,2)</f>
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="J6" s="22">
         <f t="shared" si="1"/>
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="J6" s="22">
+        <v>85480</v>
+      </c>
+      <c r="K6" s="7">
         <f t="shared" si="2"/>
-        <v>85480</v>
-      </c>
-      <c r="K6" s="7">
+        <v>14520</v>
+      </c>
+      <c r="L6" s="21">
         <f t="shared" si="3"/>
-        <v>14520</v>
-      </c>
-      <c r="L6" s="21">
+        <v>1190.6400000000001</v>
+      </c>
+      <c r="M6" s="21">
         <f t="shared" si="4"/>
-        <v>1190.6400000000001</v>
-      </c>
-      <c r="M6" s="21">
+        <v>13329.36</v>
+      </c>
+      <c r="N6" s="34">
         <f t="shared" si="5"/>
-        <v>13329.36</v>
-      </c>
-      <c r="N6" s="34">
-        <f t="shared" si="6"/>
         <v>3.4604693562421046E-2</v>
       </c>
       <c r="O6" s="23"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>2008</v>
-      </c>
-      <c r="B7">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="C7">
-        <v>0.1108</v>
-      </c>
+      <c r="A7" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
       <c r="F7" s="1">
         <v>2009</v>
       </c>
@@ -941,45 +922,41 @@
         <v>0.82699999999999996</v>
       </c>
       <c r="H7" s="14">
-        <f t="shared" si="7"/>
+        <f>VLOOKUP(F7,$A$46:$B$58,2)*0.01</f>
         <v>0.17300000000000001</v>
       </c>
       <c r="I7" s="4">
+        <f>VLOOKUP(F7,$A$18:$C$26,2)</f>
+        <v>0.1152</v>
+      </c>
+      <c r="J7" s="22">
         <f t="shared" si="1"/>
-        <v>0.1152</v>
-      </c>
-      <c r="J7" s="22">
+        <v>82700</v>
+      </c>
+      <c r="K7" s="7">
         <f t="shared" si="2"/>
-        <v>82700</v>
-      </c>
-      <c r="K7" s="7">
+        <v>17300</v>
+      </c>
+      <c r="L7" s="21">
         <f t="shared" si="3"/>
-        <v>17300</v>
-      </c>
-      <c r="L7" s="21">
+        <v>1992.96</v>
+      </c>
+      <c r="M7" s="21">
         <f t="shared" si="4"/>
-        <v>1992.96</v>
-      </c>
-      <c r="M7" s="21">
+        <v>15307.04</v>
+      </c>
+      <c r="N7" s="34">
         <f t="shared" si="5"/>
-        <v>15307.04</v>
-      </c>
-      <c r="N7" s="34">
-        <f t="shared" si="6"/>
         <v>6.0191937197284787E-2</v>
       </c>
       <c r="O7" s="23"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B8">
-        <v>0.1152</v>
-      </c>
-      <c r="C8">
-        <v>0.15570000000000001</v>
-      </c>
+        <v>1995</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
       <c r="F8" s="2">
         <v>2010</v>
       </c>
@@ -988,19 +965,19 @@
         <v>0.83389999999999997</v>
       </c>
       <c r="H8" s="14">
-        <f t="shared" si="7"/>
+        <f>VLOOKUP(F8,$A$46:$B$58,2)*0.01</f>
         <v>0.1661</v>
       </c>
       <c r="I8" s="4">
+        <f>VLOOKUP(F8,$A$18:$C$26,2)</f>
+        <v>0.1416</v>
+      </c>
+      <c r="J8" s="22">
         <f t="shared" si="1"/>
-        <v>0.1416</v>
-      </c>
-      <c r="J8" s="22">
+        <v>83390</v>
+      </c>
+      <c r="K8" s="7">
         <f t="shared" si="2"/>
-        <v>83390</v>
-      </c>
-      <c r="K8" s="7">
-        <f t="shared" si="3"/>
         <v>16610</v>
       </c>
       <c r="L8" s="21">
@@ -1008,25 +985,21 @@
         <v>2351.9760000000001</v>
       </c>
       <c r="M8" s="21">
+        <f t="shared" si="4"/>
+        <v>14258.023999999999</v>
+      </c>
+      <c r="N8" s="34">
         <f t="shared" si="5"/>
-        <v>14258.023999999999</v>
-      </c>
-      <c r="N8" s="34">
-        <f t="shared" si="6"/>
         <v>2.345430599253677E-2</v>
       </c>
       <c r="O8" s="23"/>
     </row>
     <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>2010</v>
-      </c>
-      <c r="B9">
-        <v>0.1416</v>
-      </c>
-      <c r="C9">
-        <v>0.1913</v>
-      </c>
+      <c r="A9" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
       <c r="F9" s="1">
         <v>2011</v>
       </c>
@@ -1035,31 +1008,31 @@
         <v>0.83129999999999993</v>
       </c>
       <c r="H9" s="14">
-        <f t="shared" si="7"/>
+        <f>VLOOKUP(F9,$A$46:$B$58,2)*0.01</f>
         <v>0.16870000000000002</v>
       </c>
       <c r="I9" s="4">
+        <f>VLOOKUP(F9,$A$18:$C$26,2)</f>
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="J9" s="22">
         <f t="shared" si="1"/>
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="J9" s="22">
+        <v>83130</v>
+      </c>
+      <c r="K9" s="7">
         <f t="shared" si="2"/>
-        <v>83130</v>
-      </c>
-      <c r="K9" s="7">
+        <v>16870</v>
+      </c>
+      <c r="L9" s="21">
         <f t="shared" si="3"/>
-        <v>16870</v>
-      </c>
-      <c r="L9" s="21">
+        <v>2969.12</v>
+      </c>
+      <c r="M9" s="21">
         <f t="shared" si="4"/>
-        <v>2969.12</v>
-      </c>
-      <c r="M9" s="21">
+        <v>13900.880000000001</v>
+      </c>
+      <c r="N9" s="34">
         <f t="shared" si="5"/>
-        <v>13900.880000000001</v>
-      </c>
-      <c r="N9" s="34">
-        <f t="shared" si="6"/>
         <v>4.3283978200625822E-2</v>
       </c>
       <c r="O9" s="24" t="s">
@@ -1068,14 +1041,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B10">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="C10">
-        <v>0.23780000000000001</v>
-      </c>
+        <v>1997</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
       <c r="F10" s="2">
         <v>2017</v>
       </c>
@@ -1084,31 +1053,31 @@
         <v>0.79830000000000001</v>
       </c>
       <c r="H10" s="14">
-        <f t="shared" si="7"/>
+        <f>VLOOKUP(F10,$A$46:$B$58,2)*0.01</f>
         <v>0.20170000000000002</v>
       </c>
       <c r="I10" s="4">
+        <f>VLOOKUP(F10,$A$18:$C$26,2)</f>
+        <v>0.44209999999999999</v>
+      </c>
+      <c r="J10" s="22">
         <f t="shared" si="1"/>
-        <v>0.44209999999999999</v>
-      </c>
-      <c r="J10" s="22">
+        <v>79830</v>
+      </c>
+      <c r="K10" s="7">
         <f t="shared" si="2"/>
-        <v>79830</v>
-      </c>
-      <c r="K10" s="7">
+        <v>20170</v>
+      </c>
+      <c r="L10" s="21">
         <f t="shared" si="3"/>
-        <v>20170</v>
-      </c>
-      <c r="L10" s="21">
+        <v>8917.1569999999992</v>
+      </c>
+      <c r="M10" s="21">
         <f t="shared" si="4"/>
-        <v>8917.1569999999992</v>
-      </c>
-      <c r="M10" s="21">
+        <v>11252.843000000001</v>
+      </c>
+      <c r="N10" s="34">
         <f t="shared" si="5"/>
-        <v>11252.843000000001</v>
-      </c>
-      <c r="N10" s="34">
-        <f t="shared" si="6"/>
         <v>0.42788924154442015</v>
       </c>
       <c r="O10" s="34">
@@ -1117,55 +1086,61 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>2017</v>
-      </c>
-      <c r="B11">
-        <v>0.44209999999999999</v>
-      </c>
-      <c r="C11">
-        <v>0.59750000000000003</v>
-      </c>
+      <c r="A11" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
       <c r="P12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
       <c r="F13" t="s">
         <v>7</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" ref="G13:N13" si="8">G1</f>
+        <f>G1</f>
         <v>HIV -</v>
       </c>
       <c r="H13" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f>H1</f>
         <v>HIV Prevalence</v>
       </c>
       <c r="I13" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f>I1</f>
         <v>ART coverage over time by gender </v>
       </c>
       <c r="J13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="K13" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f>K1</f>
         <v xml:space="preserve">Number of population (HIV +) </v>
       </c>
       <c r="L13" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f>L1</f>
         <v xml:space="preserve">Number of population (ART) </v>
       </c>
       <c r="M13" s="5" t="s">
         <v>32</v>
       </c>
       <c r="N13" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f>N1</f>
         <v>ART rate initiation</v>
       </c>
       <c r="P13" s="9">
@@ -1173,34 +1148,32 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A14" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A15" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
       <c r="F15" s="13">
-        <f t="shared" ref="F15:F22" si="9">F3</f>
+        <f>F3</f>
         <v>2005</v>
       </c>
       <c r="G15" s="14">
-        <f t="shared" ref="G15:G21" si="10">1-H15</f>
+        <f t="shared" ref="G15:G21" si="6">1-H15</f>
         <v>0.74509999999999998</v>
       </c>
       <c r="H15" s="14">
-        <f>VLOOKUP(F15,$A$15:$C$28,3)*0.01</f>
+        <f>VLOOKUP(F15,$A$30:$C$58,3)*0.01</f>
         <v>0.25490000000000002</v>
       </c>
       <c r="I15" s="16">
-        <f>VLOOKUP(F15,$A$3:$C$11,3)</f>
+        <f>VLOOKUP(F15,$A$18:$C$26,3)</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="J15" s="22">
@@ -1208,7 +1181,7 @@
         <v>74510</v>
       </c>
       <c r="K15" s="17">
-        <f t="shared" ref="K15:K21" si="11">$P$13*H15</f>
+        <f>$P$13*H15</f>
         <v>25490</v>
       </c>
       <c r="L15" s="20">
@@ -1222,46 +1195,42 @@
       <c r="N15" s="8"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>2005</v>
-      </c>
-      <c r="B16">
-        <v>13.83</v>
-      </c>
-      <c r="C16">
-        <v>25.49</v>
-      </c>
+      <c r="A16" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="10"/>
       <c r="F16" s="13">
-        <f t="shared" si="9"/>
+        <f>F4</f>
         <v>2006</v>
       </c>
       <c r="G16" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0.74790000000000001</v>
       </c>
       <c r="H16" s="14">
-        <f t="shared" ref="H16:H22" si="12">VLOOKUP(F16,$A$15:$C$28,3)*0.01</f>
+        <f>VLOOKUP(F16,$A$30:$C$58,3)*0.01</f>
         <v>0.25209999999999999</v>
       </c>
       <c r="I16" s="16">
-        <f t="shared" ref="I16:I22" si="13">VLOOKUP(F16,$A$3:$C$11,3)</f>
+        <f>VLOOKUP(F16,$A$18:$C$26,3)</f>
         <v>2.9399999999999999E-2</v>
       </c>
       <c r="J16" s="22">
-        <f t="shared" ref="J16:J22" si="14">$P$13-K16</f>
+        <f>$P$13-K16</f>
         <v>74790</v>
       </c>
       <c r="K16" s="17">
-        <f t="shared" si="11"/>
+        <f>$P$13*H16</f>
         <v>25210</v>
       </c>
       <c r="L16" s="20">
-        <f t="shared" ref="L16:L22" si="15">I16*K16</f>
+        <f t="shared" ref="L16:L22" si="7">I16*K16</f>
         <v>741.17399999999998</v>
       </c>
       <c r="M16" s="21">
-        <f t="shared" ref="M16:M22" si="16">K16-L16</f>
+        <f t="shared" ref="M16:M22" si="8">K16-L16</f>
         <v>24468.826000000001</v>
       </c>
       <c r="N16" s="34">
@@ -1271,46 +1240,42 @@
       <c r="O16" s="35"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>2006</v>
-      </c>
-      <c r="B17">
-        <v>13.3</v>
-      </c>
-      <c r="C17">
-        <v>25.21</v>
-      </c>
+      <c r="A17" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="10"/>
       <c r="F17" s="13">
-        <f t="shared" si="9"/>
+        <f>F5</f>
         <v>2007</v>
       </c>
       <c r="G17" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0.72589999999999999</v>
       </c>
       <c r="H17" s="14">
-        <f t="shared" si="12"/>
+        <f>VLOOKUP(F17,$A$30:$C$58,3)*0.01</f>
         <v>0.27410000000000001</v>
       </c>
       <c r="I17" s="16">
-        <f t="shared" si="13"/>
+        <f>VLOOKUP(F17,$A$18:$C$26,3)</f>
         <v>6.4299999999999996E-2</v>
       </c>
       <c r="J17" s="22">
-        <f t="shared" si="14"/>
+        <f>$P$13-K17</f>
         <v>72590</v>
       </c>
       <c r="K17" s="17">
-        <f t="shared" si="11"/>
+        <f>$P$13*H17</f>
         <v>27410</v>
       </c>
       <c r="L17" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>1762.463</v>
       </c>
       <c r="M17" s="21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="8"/>
         <v>25647.537</v>
       </c>
       <c r="N17" s="34">
@@ -1321,189 +1286,189 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="B18">
-        <v>14.78</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>27.41</v>
+        <v>0</v>
       </c>
       <c r="F18" s="13">
+        <f>F6</f>
+        <v>2008</v>
+      </c>
+      <c r="G18" s="14">
+        <f t="shared" si="6"/>
+        <v>0.71100000000000008</v>
+      </c>
+      <c r="H18" s="14">
+        <f>VLOOKUP(F18,$A$30:$C$58,3)*0.01</f>
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="I18" s="16">
+        <f>VLOOKUP(F18,$A$18:$C$26,3)</f>
+        <v>0.1108</v>
+      </c>
+      <c r="J18" s="22">
+        <f>$P$13-K18</f>
+        <v>71100</v>
+      </c>
+      <c r="K18" s="17">
+        <f>$P$13*H18</f>
+        <v>28899.999999999996</v>
+      </c>
+      <c r="L18" s="20">
+        <f t="shared" si="7"/>
+        <v>3202.1199999999994</v>
+      </c>
+      <c r="M18" s="21">
+        <f t="shared" si="8"/>
+        <v>25697.879999999997</v>
+      </c>
+      <c r="N18" s="34">
+        <f t="shared" ref="N18:N20" si="9">(L18-L17)/M17</f>
+        <v>5.6132368577926195E-2</v>
+      </c>
+      <c r="O18" s="35"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B19">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="C19">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="F19" s="13">
+        <f>F7</f>
+        <v>2009</v>
+      </c>
+      <c r="G19" s="14">
+        <f t="shared" si="6"/>
+        <v>0.68280000000000007</v>
+      </c>
+      <c r="H19" s="14">
+        <f>VLOOKUP(F19,$A$30:$C$58,3)*0.01</f>
+        <v>0.31719999999999998</v>
+      </c>
+      <c r="I19" s="16">
+        <f>VLOOKUP(F19,$A$18:$C$26,3)</f>
+        <v>0.15570000000000001</v>
+      </c>
+      <c r="J19" s="22">
+        <f>$P$13-K19</f>
+        <v>68280</v>
+      </c>
+      <c r="K19" s="17">
+        <f>$P$13*H19</f>
+        <v>31720</v>
+      </c>
+      <c r="L19" s="20">
+        <f t="shared" si="7"/>
+        <v>4938.8040000000001</v>
+      </c>
+      <c r="M19" s="21">
+        <f t="shared" si="8"/>
+        <v>26781.196</v>
+      </c>
+      <c r="N19" s="34">
         <f t="shared" si="9"/>
-        <v>2008</v>
-      </c>
-      <c r="G18" s="14">
-        <f t="shared" si="10"/>
-        <v>0.71100000000000008</v>
-      </c>
-      <c r="H18" s="14">
-        <f t="shared" si="12"/>
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="I18" s="16">
-        <f t="shared" si="13"/>
-        <v>0.1108</v>
-      </c>
-      <c r="J18" s="22">
-        <f t="shared" si="14"/>
-        <v>71100</v>
-      </c>
-      <c r="K18" s="17">
-        <f t="shared" si="11"/>
-        <v>28899.999999999996</v>
-      </c>
-      <c r="L18" s="20">
-        <f t="shared" si="15"/>
-        <v>3202.1199999999994</v>
-      </c>
-      <c r="M18" s="21">
-        <f t="shared" si="16"/>
-        <v>25697.879999999997</v>
-      </c>
-      <c r="N18" s="34">
-        <f t="shared" ref="N18:N20" si="17">(L18-L17)/M17</f>
-        <v>5.6132368577926195E-2</v>
-      </c>
-      <c r="O18" s="35"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>2008</v>
-      </c>
-      <c r="B19">
-        <v>14.52</v>
-      </c>
-      <c r="C19">
-        <v>28.9</v>
-      </c>
-      <c r="F19" s="13">
-        <f t="shared" si="9"/>
-        <v>2009</v>
-      </c>
-      <c r="G19" s="14">
-        <f t="shared" si="10"/>
-        <v>0.68280000000000007</v>
-      </c>
-      <c r="H19" s="14">
-        <f t="shared" si="12"/>
-        <v>0.31719999999999998</v>
-      </c>
-      <c r="I19" s="16">
-        <f t="shared" si="13"/>
-        <v>0.15570000000000001</v>
-      </c>
-      <c r="J19" s="22">
-        <f t="shared" si="14"/>
-        <v>68280</v>
-      </c>
-      <c r="K19" s="17">
-        <f t="shared" si="11"/>
-        <v>31720</v>
-      </c>
-      <c r="L19" s="20">
-        <f t="shared" si="15"/>
-        <v>4938.8040000000001</v>
-      </c>
-      <c r="M19" s="21">
-        <f t="shared" si="16"/>
-        <v>26781.196</v>
-      </c>
-      <c r="N19" s="34">
-        <f t="shared" si="17"/>
         <v>6.7580827679170452E-2</v>
       </c>
       <c r="O19" s="35"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="B20">
-        <v>17.3</v>
+        <v>2.18E-2</v>
       </c>
       <c r="C20">
-        <v>31.72</v>
+        <v>2.9399999999999999E-2</v>
       </c>
       <c r="D20" s="10"/>
       <c r="F20" s="13">
+        <f>F8</f>
+        <v>2010</v>
+      </c>
+      <c r="G20" s="14">
+        <f t="shared" si="6"/>
+        <v>0.65290000000000004</v>
+      </c>
+      <c r="H20" s="14">
+        <f>VLOOKUP(F20,$A$30:$C$58,3)*0.01</f>
+        <v>0.34710000000000002</v>
+      </c>
+      <c r="I20" s="16">
+        <f>VLOOKUP(F20,$A$18:$C$26,3)</f>
+        <v>0.1913</v>
+      </c>
+      <c r="J20" s="22">
+        <f>$P$13-K20</f>
+        <v>65290</v>
+      </c>
+      <c r="K20" s="17">
+        <f>$P$13*H20</f>
+        <v>34710</v>
+      </c>
+      <c r="L20" s="20">
+        <f t="shared" si="7"/>
+        <v>6640.0230000000001</v>
+      </c>
+      <c r="M20" s="21">
+        <f t="shared" si="8"/>
+        <v>28069.976999999999</v>
+      </c>
+      <c r="N20" s="34">
         <f t="shared" si="9"/>
-        <v>2010</v>
-      </c>
-      <c r="G20" s="14">
-        <f t="shared" si="10"/>
-        <v>0.65290000000000004</v>
-      </c>
-      <c r="H20" s="14">
-        <f t="shared" si="12"/>
-        <v>0.34710000000000002</v>
-      </c>
-      <c r="I20" s="16">
-        <f t="shared" si="13"/>
-        <v>0.1913</v>
-      </c>
-      <c r="J20" s="22">
-        <f t="shared" si="14"/>
-        <v>65290</v>
-      </c>
-      <c r="K20" s="17">
-        <f t="shared" si="11"/>
-        <v>34710</v>
-      </c>
-      <c r="L20" s="20">
-        <f t="shared" si="15"/>
-        <v>6640.0230000000001</v>
-      </c>
-      <c r="M20" s="21">
-        <f t="shared" si="16"/>
-        <v>28069.976999999999</v>
-      </c>
-      <c r="N20" s="34">
-        <f t="shared" si="17"/>
         <v>6.3522891210683802E-2</v>
       </c>
       <c r="O20" s="35"/>
     </row>
     <row r="21" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>2010</v>
-      </c>
-      <c r="B21">
-        <v>16.61</v>
+      <c r="A21" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B21" s="3">
+        <v>4.7600000000000003E-2</v>
       </c>
       <c r="C21">
-        <v>34.71</v>
+        <v>6.4299999999999996E-2</v>
       </c>
       <c r="F21" s="13">
-        <f t="shared" si="9"/>
+        <f>F9</f>
         <v>2011</v>
       </c>
       <c r="G21" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0.64860000000000007</v>
       </c>
       <c r="H21" s="14">
-        <f t="shared" si="12"/>
+        <f>VLOOKUP(F21,$A$30:$C$58,3)*0.01</f>
         <v>0.35139999999999999</v>
       </c>
       <c r="I21" s="16">
-        <f t="shared" si="13"/>
+        <f>VLOOKUP(F21,$A$18:$C$26,3)</f>
         <v>0.23780000000000001</v>
       </c>
       <c r="J21" s="22">
-        <f t="shared" si="14"/>
+        <f>$P$13-K21</f>
         <v>64860</v>
       </c>
       <c r="K21" s="17">
-        <f t="shared" si="11"/>
+        <f>$P$13*H21</f>
         <v>35140</v>
       </c>
       <c r="L21" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>8356.2920000000013</v>
       </c>
       <c r="M21" s="21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="8"/>
         <v>26783.707999999999</v>
       </c>
       <c r="N21" s="34">
@@ -1516,16 +1481,16 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="B22">
-        <v>16.87</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="C22">
-        <v>35.14</v>
+        <v>0.1108</v>
       </c>
       <c r="F22" s="13">
-        <f t="shared" si="9"/>
+        <f>F10</f>
         <v>2017</v>
       </c>
       <c r="G22" s="14">
@@ -1533,15 +1498,15 @@
         <v>0.59549999999999992</v>
       </c>
       <c r="H22" s="14">
-        <f t="shared" si="12"/>
+        <f>VLOOKUP(F22,$A$30:$C$58,3)*0.01</f>
         <v>0.40450000000000003</v>
       </c>
       <c r="I22" s="16">
-        <f t="shared" si="13"/>
+        <f>VLOOKUP(F22,$A$18:$C$26,3)</f>
         <v>0.59750000000000003</v>
       </c>
       <c r="J22" s="22">
-        <f t="shared" si="14"/>
+        <f>$P$13-K22</f>
         <v>59550</v>
       </c>
       <c r="K22" s="17">
@@ -1549,11 +1514,11 @@
         <v>40450</v>
       </c>
       <c r="L22" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>24168.875</v>
       </c>
       <c r="M22" s="21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="8"/>
         <v>16281.125</v>
       </c>
       <c r="N22" s="34">
@@ -1566,14 +1531,14 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>2012</v>
+      <c r="A23" s="1">
+        <v>2009</v>
       </c>
       <c r="B23">
-        <v>17.48</v>
+        <v>0.1152</v>
       </c>
       <c r="C23">
-        <v>36.19</v>
+        <v>0.15570000000000001</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
@@ -1586,109 +1551,331 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="B24">
-        <v>19.13</v>
+        <v>0.1416</v>
       </c>
       <c r="C24">
-        <v>38.119999999999997</v>
+        <v>0.1913</v>
       </c>
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>2014</v>
+      <c r="A25" s="1">
+        <v>2011</v>
       </c>
       <c r="B25">
-        <v>20.87</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="C25">
-        <v>40.76</v>
+        <v>0.23780000000000001</v>
       </c>
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B26">
+        <v>0.44209999999999999</v>
+      </c>
+      <c r="C26">
+        <v>0.59750000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="F40" s="13"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="F41" s="13"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="F42" s="13"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="F45" s="13"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B46">
+        <v>13.83</v>
+      </c>
+      <c r="C46">
+        <v>25.49</v>
+      </c>
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B47">
+        <v>13.3</v>
+      </c>
+      <c r="C47">
+        <v>25.21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B48">
+        <v>14.78</v>
+      </c>
+      <c r="C48">
+        <v>27.41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B49">
+        <v>14.52</v>
+      </c>
+      <c r="C49">
+        <v>28.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B50">
+        <v>17.3</v>
+      </c>
+      <c r="C50">
+        <v>31.72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B51">
+        <v>16.61</v>
+      </c>
+      <c r="C51">
+        <v>34.71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B52">
+        <v>16.87</v>
+      </c>
+      <c r="C52">
+        <v>35.14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B53">
+        <v>17.48</v>
+      </c>
+      <c r="C53">
+        <v>36.19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B54">
+        <v>19.13</v>
+      </c>
+      <c r="C54">
+        <v>38.119999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B55">
+        <v>20.87</v>
+      </c>
+      <c r="C55">
+        <v>40.76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
         <v>2015</v>
       </c>
-      <c r="B26">
+      <c r="B56">
         <v>18.96</v>
       </c>
-      <c r="C26">
+      <c r="C56">
         <v>41.81</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
         <v>2016</v>
       </c>
-      <c r="B27">
+      <c r="B57">
         <v>19.91</v>
       </c>
-      <c r="C27">
+      <c r="C57">
         <v>42.06</v>
       </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
         <v>2017</v>
       </c>
-      <c r="B28">
+      <c r="B58">
         <v>20.170000000000002</v>
       </c>
-      <c r="C28">
+      <c r="C58">
         <v>40.450000000000003</v>
       </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="11"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="2"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="12"/>
-      <c r="F39" s="13"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F40" s="13"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F41" s="13"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F42" s="13"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F43" s="13"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F44" s="13"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F45" s="13"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F46" s="13"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B63" s="11"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="11"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1700,7 +1887,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>